<commit_message>
Last update on Excel table
</commit_message>
<xml_diff>
--- a/ARN Table.xlsx
+++ b/ARN Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Perso\Formations\THP\Developpeur_24_semaines\W8\W8D4\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{432E064C-0B9B-4C07-89FE-E8844F83EE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5934DBC2-F7D1-4A7F-946F-F357A8D1D94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4"/>
   </bookViews>
@@ -5213,8 +5213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D65" sqref="D2:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>